<commit_message>
Aggiornato Test Indicatori ISPRO
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.monaco\Desktop\ISP\SorgentiGIT\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="casistiche Indeterm" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="OUTPUT" sheetId="8" r:id="rId4"/>
     <sheet name="Query" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="150">
   <si>
     <t>SNDG</t>
   </si>
@@ -528,12 +528,72 @@
   <si>
     <t>EST000010</t>
   </si>
+  <si>
+    <t>EST000016</t>
+  </si>
+  <si>
+    <t>EST000035</t>
+  </si>
+  <si>
+    <t>EST000005</t>
+  </si>
+  <si>
+    <t>EST000022</t>
+  </si>
+  <si>
+    <t>EST000013</t>
+  </si>
+  <si>
+    <t>EST000004</t>
+  </si>
+  <si>
+    <t>EST000027</t>
+  </si>
+  <si>
+    <t>EST000021</t>
+  </si>
+  <si>
+    <t>EST000001</t>
+  </si>
+  <si>
+    <t>EST000030</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>EST000033</t>
+  </si>
+  <si>
+    <t>EST000014</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>EST000044</t>
+  </si>
+  <si>
+    <t>EST000009</t>
+  </si>
+  <si>
+    <t>EST000046</t>
+  </si>
+  <si>
+    <t>Il Max è 180</t>
+  </si>
+  <si>
+    <t>Il numero di giorni non può essere negativo</t>
+  </si>
+  <si>
+    <t>Note KO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +659,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -716,7 +784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -775,14 +843,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1113,19 +1187,19 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="24"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1133,13 +1207,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1224,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
@@ -1159,7 +1233,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -1168,7 +1242,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1177,7 +1251,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -1186,7 +1260,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -1195,7 +1269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>8</v>
@@ -1204,7 +1278,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -1213,13 +1287,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="24"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1227,19 +1301,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -1262,19 +1336,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="112.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="6.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="112.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>4</v>
       </c>
@@ -1282,7 +1356,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>5</v>
       </c>
@@ -1290,7 +1364,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>19</v>
       </c>
@@ -1298,7 +1372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>23</v>
       </c>
@@ -1306,7 +1380,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>24</v>
       </c>
@@ -1314,7 +1388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="17">
         <v>31</v>
       </c>
@@ -1322,7 +1396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>45</v>
       </c>
@@ -1330,7 +1404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>52</v>
       </c>
@@ -1338,7 +1412,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>57</v>
       </c>
@@ -1346,7 +1420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>176</v>
       </c>
@@ -1354,7 +1428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
         <v>178</v>
       </c>
@@ -1362,7 +1436,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="17">
         <v>179</v>
       </c>
@@ -1370,7 +1444,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>184</v>
       </c>
@@ -1378,7 +1452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="17">
         <v>185</v>
       </c>
@@ -1395,33 +1469,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="19.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="21" width="9.109375" style="7"/>
+    <col min="9" max="9" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>26</v>
       </c>
@@ -1444,8 +1518,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
@@ -1461,8 +1537,10 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1478,8 +1556,10 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
@@ -1499,12 +1579,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
@@ -1529,8 +1609,10 @@
       <c r="T8"/>
       <c r="U8"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1548,8 +1630,10 @@
       <c r="T9"/>
       <c r="U9"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B10" s="1">
         <v>0</v>
       </c>
@@ -1571,8 +1655,10 @@
       <c r="T10"/>
       <c r="U10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1590,8 +1676,10 @@
       <c r="T11"/>
       <c r="U11"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
@@ -1613,12 +1701,12 @@
       <c r="T12"/>
       <c r="U12"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -1641,8 +1729,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
@@ -1658,8 +1748,10 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
@@ -1675,8 +1767,10 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B18" s="1">
         <v>0</v>
       </c>
@@ -1696,12 +1790,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>26</v>
       </c>
@@ -1724,8 +1818,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
@@ -1741,8 +1837,10 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
@@ -1758,8 +1856,10 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
@@ -1777,12 +1877,12 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>26</v>
       </c>
@@ -1805,8 +1905,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
@@ -1822,8 +1924,10 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
@@ -1839,8 +1943,10 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
@@ -1858,12 +1964,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="25"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J32" s="25"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>26</v>
       </c>
@@ -1888,122 +1998,168 @@
       <c r="H33" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J33" s="23"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+      <c r="J33" s="25"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="25">
+      <c r="D34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="23">
         <v>42735</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="23">
         <v>42674</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
       <c r="H34" s="1"/>
-      <c r="J34" s="23"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
+      <c r="J34" s="25"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="25">
+      <c r="D35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="23">
         <v>42735</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="23">
         <v>42369</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
       <c r="H35" s="1"/>
-      <c r="J35" s="23"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+      <c r="J35" s="25"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="25">
+      <c r="D36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="23">
         <v>42735</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="23">
         <v>42645</v>
       </c>
-      <c r="G36" s="1"/>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
       <c r="H36" s="1"/>
-      <c r="J36" s="23"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1" t="s">
-        <v>23</v>
+      <c r="J36" s="25"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="J37" s="23"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1" t="s">
-        <v>23</v>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="25"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="25">
+      <c r="F38" s="23">
         <v>42735</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="J38" s="23"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1" t="s">
-        <v>23</v>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J38" s="25"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="25">
+      <c r="D39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="23">
         <v>42735</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="J39" s="23"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="25"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="25"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J41" s="25"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>26</v>
       </c>
@@ -2025,9 +2181,12 @@
       <c r="G42" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
+      <c r="J42" s="25"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B43" s="1">
         <v>0</v>
       </c>
@@ -2042,9 +2201,12 @@
         <v>0</v>
       </c>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
+      <c r="J43" s="25"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B44" s="1">
         <v>1</v>
       </c>
@@ -2060,8 +2222,10 @@
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B45" s="1">
         <v>0</v>
       </c>
@@ -2081,12 +2245,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>26</v>
       </c>
@@ -2109,8 +2273,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B49" s="1">
         <v>0</v>
       </c>
@@ -2126,8 +2292,10 @@
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B50" s="1">
         <v>1</v>
       </c>
@@ -2143,8 +2311,10 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B51" s="1">
         <v>0</v>
       </c>
@@ -2163,13 +2333,18 @@
       <c r="G51" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J51" s="25"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J52" s="25"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J53" s="25"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>26</v>
       </c>
@@ -2194,156 +2369,222 @@
       <c r="H54" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J54" s="23"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
+      <c r="J54" s="25"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B55" s="1">
         <v>180</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="E55" s="1">
         <v>180</v>
       </c>
       <c r="F55" s="1">
         <v>120</v>
       </c>
-      <c r="G55" s="1"/>
+      <c r="G55" s="1">
+        <v>180</v>
+      </c>
       <c r="H55" s="1"/>
-      <c r="J55" s="23"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
+      <c r="J55" s="25"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B56" s="1">
         <v>80</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="E56" s="1">
         <v>20</v>
       </c>
       <c r="F56" s="1">
         <v>80</v>
       </c>
-      <c r="G56" s="1"/>
+      <c r="G56" s="1">
+        <v>80</v>
+      </c>
       <c r="H56" s="1"/>
-      <c r="J56" s="23"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
+      <c r="J56" s="25"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B57" s="1">
         <v>30</v>
       </c>
       <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="E57" s="1">
         <v>30</v>
       </c>
       <c r="F57" s="1">
         <v>30</v>
       </c>
-      <c r="G57" s="1"/>
+      <c r="G57" s="1">
+        <v>30</v>
+      </c>
       <c r="H57" s="1"/>
-      <c r="J57" s="23"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
-        <v>23</v>
+      <c r="J57" s="25"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="J58" s="23"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J58" s="25"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B59" s="1">
         <v>20</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F59" s="1">
         <v>20</v>
       </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="J59" s="23"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1">
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J59" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="26">
         <v>180</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1">
+      <c r="C60" s="26"/>
+      <c r="D60" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E60" s="26">
         <v>180</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="J60" s="23"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1">
+      <c r="F60" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" s="26">
+        <v>0</v>
+      </c>
+      <c r="H60" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J60" s="27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="26">
+        <v>0</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" s="26">
         <v>-10</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="26">
         <v>20</v>
       </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="J61" s="23"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1">
+      <c r="G61" s="26">
         <v>20</v>
       </c>
-      <c r="F62" s="1">
+      <c r="H61" s="26"/>
+      <c r="J61" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="26">
+        <v>0</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E62" s="26">
+        <v>20</v>
+      </c>
+      <c r="F62" s="26">
         <v>-50</v>
       </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="J62" s="23"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G62" s="26">
+        <v>20</v>
+      </c>
+      <c r="H62" s="26"/>
+      <c r="J62" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J63" s="25"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J64" s="25"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>26</v>
       </c>
@@ -2365,54 +2606,75 @@
       <c r="G65" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
+      <c r="J65" s="25"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B66" s="1">
         <v>0</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="E66" s="1">
         <v>0</v>
       </c>
-      <c r="F66" s="1"/>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B67" s="1">
         <v>1</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="D67" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E67" s="1">
         <v>1</v>
       </c>
-      <c r="F67" s="1"/>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B68" s="1">
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B70" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>26</v>
       </c>
@@ -2438,7 +2700,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1">
         <v>9</v>
@@ -2454,7 +2716,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1">
         <v>0.25</v>
@@ -2470,7 +2732,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
         <v>23</v>
@@ -2488,7 +2750,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
         <v>23</v>
@@ -2506,7 +2768,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
         <v>23</v>
@@ -2524,7 +2786,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
         <v>23</v>
@@ -2542,7 +2804,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
         <v>23</v>
@@ -2560,7 +2822,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
         <v>23</v>
@@ -2578,7 +2840,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
         <v>23</v>
@@ -2596,7 +2858,7 @@
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
         <v>23</v>
@@ -2614,12 +2876,12 @@
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>26</v>
       </c>
@@ -2645,7 +2907,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1">
         <v>9</v>
@@ -2661,7 +2923,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1">
         <v>0.25</v>
@@ -2677,7 +2939,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
         <v>23</v>
@@ -2695,7 +2957,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1" t="s">
         <v>23</v>
@@ -2713,7 +2975,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
         <v>23</v>
@@ -2731,7 +2993,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1" t="s">
         <v>23</v>
@@ -2749,7 +3011,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1" t="s">
         <v>23</v>
@@ -2767,7 +3029,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1" t="s">
         <v>23</v>
@@ -2785,7 +3047,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1" t="s">
         <v>23</v>
@@ -2803,7 +3065,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1" t="s">
         <v>23</v>
@@ -2821,12 +3083,12 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B96" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>26</v>
       </c>
@@ -2852,7 +3114,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1">
         <v>9</v>
@@ -2868,7 +3130,7 @@
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1">
         <v>0.25</v>
@@ -2884,7 +3146,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1" t="s">
         <v>23</v>
@@ -2902,7 +3164,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
         <v>23</v>
@@ -2920,7 +3182,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1" t="s">
         <v>23</v>
@@ -2938,7 +3200,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1" t="s">
         <v>23</v>
@@ -2956,7 +3218,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1" t="s">
         <v>23</v>
@@ -2974,7 +3236,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1" t="s">
         <v>23</v>
@@ -2992,7 +3254,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1" t="s">
         <v>23</v>
@@ -3010,7 +3272,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1" t="s">
         <v>23</v>
@@ -3028,12 +3290,12 @@
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
         <v>26</v>
       </c>
@@ -3059,7 +3321,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1">
         <v>9</v>
@@ -3075,7 +3337,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1">
         <v>0.25</v>
@@ -3091,7 +3353,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1" t="s">
         <v>23</v>
@@ -3109,7 +3371,7 @@
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1" t="s">
         <v>23</v>
@@ -3127,7 +3389,7 @@
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1" t="s">
         <v>23</v>
@@ -3145,7 +3407,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1" t="s">
         <v>23</v>
@@ -3163,7 +3425,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1" t="s">
         <v>23</v>
@@ -3181,7 +3443,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1" t="s">
         <v>23</v>
@@ -3199,7 +3461,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1" t="s">
         <v>23</v>
@@ -3217,7 +3479,7 @@
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1" t="s">
         <v>23</v>
@@ -3249,18 +3511,18 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="13"/>
+    <col min="7" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E1" s="21" t="s">
         <v>115</v>
       </c>
@@ -3268,7 +3530,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>83</v>
       </c>
@@ -3285,7 +3547,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>97</v>
       </c>
@@ -3298,7 +3560,7 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>99</v>
       </c>
@@ -3311,7 +3573,7 @@
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>100</v>
       </c>
@@ -3324,7 +3586,7 @@
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>84</v>
       </c>
@@ -3337,7 +3599,7 @@
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>102</v>
       </c>
@@ -3350,7 +3612,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>85</v>
       </c>
@@ -3363,7 +3625,7 @@
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>86</v>
       </c>
@@ -3376,7 +3638,7 @@
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>106</v>
       </c>
@@ -3389,7 +3651,7 @@
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>108</v>
       </c>
@@ -3402,7 +3664,7 @@
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>119</v>
       </c>
@@ -3415,7 +3677,7 @@
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>120</v>
       </c>
@@ -3428,7 +3690,7 @@
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>89</v>
       </c>
@@ -3441,7 +3703,7 @@
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>89</v>
       </c>
@@ -3454,7 +3716,7 @@
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>89</v>
       </c>
@@ -3467,7 +3729,7 @@
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>89</v>
       </c>
@@ -3480,7 +3742,7 @@
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>89</v>
       </c>
@@ -3493,7 +3755,7 @@
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>89</v>
       </c>
@@ -3519,16 +3781,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="8.85546875" style="3"/>
     <col min="2" max="2" width="68" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="89.44140625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="46.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="89.42578125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
@@ -3542,7 +3804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Aggiornamento file test ISPRO
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="164">
   <si>
     <t>SNDG</t>
   </si>
@@ -605,6 +605,30 @@
   </si>
   <si>
     <t>Corretto senza val_max</t>
+  </si>
+  <si>
+    <t>EST000048</t>
+  </si>
+  <si>
+    <t>EST000025</t>
+  </si>
+  <si>
+    <t>EST000036</t>
+  </si>
+  <si>
+    <t>EST000028</t>
+  </si>
+  <si>
+    <t>EST000038</t>
+  </si>
+  <si>
+    <t>EST000023</t>
+  </si>
+  <si>
+    <t>EST000019</t>
+  </si>
+  <si>
+    <t>EST000050</t>
   </si>
 </sst>
 </file>
@@ -889,13 +913,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1234,10 +1258,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -1328,10 +1352,10 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -1509,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,28 +2765,28 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="B72" s="29">
+      <c r="A72" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="28">
         <v>0.73400659999999995</v>
       </c>
-      <c r="C72" s="29"/>
-      <c r="D72" s="29" t="s">
+      <c r="C72" s="28"/>
+      <c r="D72" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="E72" s="29">
+      <c r="E72" s="28">
         <v>180000</v>
       </c>
-      <c r="F72" s="29">
+      <c r="F72" s="28">
         <v>20000</v>
       </c>
-      <c r="G72" s="29">
+      <c r="G72" s="28">
         <v>9</v>
       </c>
-      <c r="H72" s="29"/>
-      <c r="I72" s="30"/>
-      <c r="J72" s="30" t="s">
+      <c r="H72" s="28"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2967,7 +2991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>143</v>
       </c>
@@ -2993,12 +3017,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B83" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>26</v>
       </c>
@@ -3024,221 +3048,309 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" s="28">
         <v>1</v>
       </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1">
+      <c r="C85" s="28"/>
+      <c r="D85" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E85" s="28">
         <v>180000</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F85" s="28">
         <v>20000</v>
       </c>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
+      <c r="G85" s="28">
+        <v>9</v>
+      </c>
+      <c r="H85" s="28"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B86" s="1">
         <v>0.25</v>
       </c>
       <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="E86" s="1">
         <v>20000</v>
       </c>
       <c r="F86" s="1">
         <v>80000</v>
       </c>
-      <c r="G86" s="1"/>
+      <c r="G86" s="1">
+        <v>0.25</v>
+      </c>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B87" s="1">
         <f>E87/F87</f>
         <v>1.25E-3</v>
       </c>
       <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="E87" s="1">
         <v>100</v>
       </c>
       <c r="F87" s="1">
         <v>80000</v>
       </c>
-      <c r="G87" s="1"/>
+      <c r="G87" s="1">
+        <v>1.25E-3</v>
+      </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" s="25">
         <v>9.2259999999999998E-4</v>
       </c>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1">
+      <c r="C88" s="25"/>
+      <c r="D88" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E88" s="25">
         <v>5</v>
       </c>
-      <c r="F88" s="1">
+      <c r="F88" s="25">
         <v>80000</v>
       </c>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
+      <c r="G88" s="25">
+        <v>6.2000000000000003E-5</v>
+      </c>
+      <c r="H88" s="25"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B89" s="27">
         <v>0.173903</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="E89" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
+      <c r="G89" s="1">
+        <v>0.173903</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B90" s="27">
         <v>0.173903</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D90" s="1"/>
+      <c r="D90" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E90" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F90" s="1">
         <v>20000</v>
       </c>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
+      <c r="G90" s="1">
+        <v>0.173903</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B91" s="27">
         <v>0.173903</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="E91" s="1">
         <v>180000</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="27">
+      <c r="G91" s="1">
         <v>0.173903</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1">
+      <c r="H91" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" s="25">
+        <v>0.173903</v>
+      </c>
+      <c r="C92" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E92" s="25">
         <v>-10000</v>
       </c>
-      <c r="F92" s="1">
+      <c r="F92" s="25">
         <v>20000</v>
       </c>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="27">
+      <c r="G92" s="25">
+        <v>-0.5</v>
+      </c>
+      <c r="H92" s="25"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" s="25">
         <v>0.173903</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1">
+      <c r="C93" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E93" s="25">
         <v>20000</v>
       </c>
-      <c r="F93" s="1">
+      <c r="F93" s="25">
         <v>-50000</v>
       </c>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
+      <c r="G93" s="25">
+        <v>-0.4</v>
+      </c>
+      <c r="H93" s="25"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B94" s="27">
         <v>0.173903</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D94" s="1"/>
+      <c r="D94" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="E94" s="1">
         <v>20000</v>
       </c>
       <c r="F94" s="1">
         <v>0</v>
       </c>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
+      <c r="G94" s="1">
+        <v>0.173903</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B95" s="27">
         <v>0.173903</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="E95" s="1">
         <v>0</v>
       </c>
       <c r="F95" s="1">
         <v>0</v>
       </c>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
+      <c r="G95" s="1">
+        <v>0.173903</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B96" s="27">
         <v>0.173903</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D96" s="1"/>
+      <c r="D96" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="E96" s="1">
         <v>0</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G96" s="1">
+        <v>0.173903</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B98" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>26</v>
       </c>
@@ -3264,204 +3376,286 @@
         <v>53</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100" s="28">
         <v>0.57777780000000001</v>
       </c>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1">
+      <c r="C100" s="28"/>
+      <c r="D100" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E100" s="28">
         <v>180000</v>
       </c>
-      <c r="F100" s="1">
+      <c r="F100" s="28">
         <v>20000</v>
       </c>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1">
+      <c r="G100" s="28">
+        <v>9</v>
+      </c>
+      <c r="H100" s="28"/>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B101" s="25">
         <v>0.25</v>
       </c>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1">
+      <c r="C101" s="25"/>
+      <c r="D101" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E101" s="25">
         <v>20000</v>
       </c>
-      <c r="F101" s="1">
+      <c r="F101" s="25">
         <v>80000</v>
       </c>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1">
+      <c r="G101" s="25">
+        <v>0</v>
+      </c>
+      <c r="H101" s="25"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B102" s="25">
         <v>3.8168E-3</v>
       </c>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1">
+      <c r="C102" s="25"/>
+      <c r="D102" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E102" s="25">
         <v>100</v>
       </c>
-      <c r="F102" s="1">
+      <c r="F102" s="25">
         <v>80000</v>
       </c>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
+      <c r="G102" s="25">
+        <v>0</v>
+      </c>
+      <c r="H102" s="25"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B103" s="27">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D103" s="1"/>
+      <c r="D103" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="E103" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
+      <c r="G103" s="1">
+        <v>6.3829800000000006E-2</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B104" s="27">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D104" s="1"/>
+      <c r="D104" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="E104" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F104" s="1">
         <v>20000</v>
       </c>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
+      <c r="G104" s="1">
+        <v>6.3829800000000006E-2</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B105" s="27">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D105" s="1"/>
+      <c r="D105" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="E105" s="1">
         <v>180000</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="27">
+      <c r="G105" s="1">
         <v>6.3829800000000006E-2</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1">
+      <c r="H105" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B106" s="25">
+        <v>6.3829800000000006E-2</v>
+      </c>
+      <c r="C106" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E106" s="25">
         <v>-10000</v>
       </c>
-      <c r="F106" s="1">
+      <c r="F106" s="25">
         <v>20000</v>
       </c>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="27">
+      <c r="G106" s="25">
+        <v>0</v>
+      </c>
+      <c r="H106" s="25"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B107" s="25">
         <v>6.3829800000000006E-2</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1">
+      <c r="C107" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D107" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E107" s="25">
         <v>20000</v>
       </c>
-      <c r="F107" s="1">
+      <c r="F107" s="25">
         <v>-50000</v>
       </c>
-      <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
+      <c r="G107" s="25">
+        <v>0</v>
+      </c>
+      <c r="H107" s="25"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B108" s="27">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D108" s="1"/>
+      <c r="D108" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="E108" s="1">
         <v>20000</v>
       </c>
       <c r="F108" s="1">
         <v>0</v>
       </c>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
+      <c r="G108" s="1">
+        <v>6.3829800000000006E-2</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B109" s="27">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D109" s="1"/>
+      <c r="D109" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="E109" s="1">
         <v>0</v>
       </c>
       <c r="F109" s="1">
         <v>0</v>
       </c>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
+      <c r="G109" s="1">
+        <v>6.3829800000000006E-2</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B110" s="27">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D110" s="1"/>
+      <c r="D110" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="E110" s="1">
         <v>0</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G110" s="1">
+        <v>6.3829800000000006E-2</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B112" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>26</v>
       </c>
@@ -3487,23 +3681,27 @@
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="28"/>
+      <c r="B114" s="28">
         <v>2.5862069999999999</v>
       </c>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1">
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28">
         <v>180000</v>
       </c>
-      <c r="F114" s="1">
+      <c r="F114" s="28">
         <v>20000</v>
       </c>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G114" s="28"/>
+      <c r="H114" s="28"/>
+      <c r="I114" s="29"/>
+      <c r="J114" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1">
         <v>0.25</v>
@@ -3519,7 +3717,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1">
         <v>2.0833299999999999E-2</v>
@@ -3535,7 +3733,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="27">
         <v>0.2368421</v>
@@ -3553,7 +3751,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="27">
         <v>0.2368421</v>
@@ -3571,7 +3769,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="27">
         <v>0.2368421</v>
@@ -3589,7 +3787,7 @@
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="27">
         <v>0.2368421</v>
@@ -3607,7 +3805,7 @@
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="27">
         <v>0.2368421</v>
@@ -3625,7 +3823,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="27">
         <v>0.2368421</v>
@@ -3643,7 +3841,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="27">
         <v>0.2368421</v>
@@ -3661,7 +3859,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="27">
         <v>0.2368421</v>

</xml_diff>

<commit_message>
Aggiornamento File Test Indicatori ISPRO
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="165">
   <si>
     <t>SNDG</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t>EST000050</t>
+  </si>
+  <si>
+    <t>EST000034</t>
   </si>
 </sst>
 </file>
@@ -1533,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I127" sqref="I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,19 +3685,25 @@
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="28"/>
+      <c r="A114" s="28" t="s">
+        <v>143</v>
+      </c>
       <c r="B114" s="28">
         <v>2.5862069999999999</v>
       </c>
       <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
+      <c r="D114" s="28" t="s">
+        <v>153</v>
+      </c>
       <c r="E114" s="28">
         <v>180000</v>
       </c>
       <c r="F114" s="28">
         <v>20000</v>
       </c>
-      <c r="G114" s="28"/>
+      <c r="G114" s="28">
+        <v>9</v>
+      </c>
       <c r="H114" s="28"/>
       <c r="I114" s="29"/>
       <c r="J114" s="29" t="s">
@@ -3702,180 +3711,252 @@
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1">
+      <c r="A115" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B115" s="25">
         <v>0.25</v>
       </c>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1">
+      <c r="C115" s="25"/>
+      <c r="D115" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E115" s="25">
         <v>20000</v>
       </c>
-      <c r="F115" s="1">
+      <c r="F115" s="25">
         <v>80000</v>
       </c>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
+      <c r="G115" s="25">
+        <v>0</v>
+      </c>
+      <c r="H115" s="25"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1">
+      <c r="A116" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B116" s="25">
         <v>2.0833299999999999E-2</v>
       </c>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1">
+      <c r="C116" s="25"/>
+      <c r="D116" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="E116" s="25">
         <v>100</v>
       </c>
-      <c r="F116" s="1">
+      <c r="F116" s="25">
         <v>80000</v>
       </c>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
+      <c r="G116" s="25">
+        <v>0</v>
+      </c>
+      <c r="H116" s="25"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
+      <c r="A117" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B117" s="27">
         <v>0.2368421</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D117" s="1"/>
+      <c r="D117" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="E117" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G117" s="1"/>
-      <c r="H117" s="1"/>
+      <c r="G117" s="1">
+        <v>0.2368421</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
+      <c r="A118" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B118" s="27">
         <v>0.2368421</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D118" s="1"/>
+      <c r="D118" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="E118" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F118" s="1">
         <v>20000</v>
       </c>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
+      <c r="G118" s="1">
+        <v>0.2368421</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
+      <c r="A119" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B119" s="27">
         <v>0.2368421</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D119" s="1"/>
+      <c r="D119" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="E119" s="1">
         <v>180000</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
+      <c r="G119" s="1">
+        <v>0.2368421</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-      <c r="B120" s="27">
+      <c r="A120" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B120" s="25">
         <v>0.2368421</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D120" s="1"/>
-      <c r="E120" s="1">
+      <c r="C120" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E120" s="25">
         <v>-10000</v>
       </c>
-      <c r="F120" s="1">
+      <c r="F120" s="25">
         <v>20000</v>
       </c>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
+      <c r="G120" s="25">
+        <v>0</v>
+      </c>
+      <c r="H120" s="25"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-      <c r="B121" s="27">
+      <c r="A121" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B121" s="25">
         <v>0.2368421</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1">
+      <c r="C121" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D121" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E121" s="25">
         <v>20000</v>
       </c>
-      <c r="F121" s="1">
+      <c r="F121" s="25">
         <v>-50000</v>
       </c>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
+      <c r="G121" s="25">
+        <v>0</v>
+      </c>
+      <c r="H121" s="25"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
+      <c r="A122" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B122" s="27">
         <v>0.2368421</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D122" s="1"/>
+      <c r="D122" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="E122" s="1">
         <v>20000</v>
       </c>
       <c r="F122" s="1">
         <v>0</v>
       </c>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
+      <c r="G122" s="1">
+        <v>0.2368421</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
+      <c r="A123" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B123" s="27">
         <v>0.2368421</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D123" s="1"/>
+      <c r="D123" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="E123" s="1">
         <v>0</v>
       </c>
       <c r="F123" s="1">
         <v>0</v>
       </c>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
+      <c r="G123" s="1">
+        <v>0.2368421</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="B124" s="27">
         <v>0.2368421</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D124" s="1"/>
+      <c r="D124" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="E124" s="1">
         <v>0</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
+      <c r="G124" s="1">
+        <v>0.2368421</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AFU e test ispro
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alberto.collu\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.monaco\Desktop\ISP\SorgentiGIT\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="casistiche Indeterm" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="165">
   <si>
     <t>SNDG</t>
   </si>
@@ -626,6 +626,12 @@
   </si>
   <si>
     <t>Exception 2</t>
+  </si>
+  <si>
+    <t>Il Max è 20</t>
+  </si>
+  <si>
+    <t>forma determinata</t>
   </si>
 </sst>
 </file>
@@ -718,7 +724,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,6 +785,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -836,7 +848,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -918,6 +930,12 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1249,19 +1267,19 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="31"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1269,13 +1287,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1304,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
@@ -1295,7 +1313,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -1304,7 +1322,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1313,7 +1331,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -1322,7 +1340,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -1331,7 +1349,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>8</v>
@@ -1340,7 +1358,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -1349,13 +1367,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="31" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1363,19 +1381,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -1394,23 +1412,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="112.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="14"/>
+    <col min="1" max="1" width="6.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="112.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>4</v>
       </c>
@@ -1418,7 +1434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>5</v>
       </c>
@@ -1426,7 +1442,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>19</v>
       </c>
@@ -1434,7 +1450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>23</v>
       </c>
@@ -1442,7 +1458,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>24</v>
       </c>
@@ -1450,7 +1466,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>31</v>
       </c>
@@ -1458,7 +1474,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>45</v>
       </c>
@@ -1466,7 +1482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>52</v>
       </c>
@@ -1474,7 +1490,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>57</v>
       </c>
@@ -1482,7 +1498,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>176</v>
       </c>
@@ -1490,7 +1506,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>178</v>
       </c>
@@ -1498,7 +1514,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>179</v>
       </c>
@@ -1506,7 +1522,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>184</v>
       </c>
@@ -1514,7 +1530,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>185</v>
       </c>
@@ -1531,33 +1547,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I127" sqref="I127"/>
+    <sheetView topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="21" width="9.140625" style="7"/>
+    <col min="9" max="9" width="19.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="19.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>26</v>
       </c>
@@ -1580,7 +1596,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>140</v>
       </c>
@@ -1599,7 +1615,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
@@ -1618,7 +1634,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>140</v>
       </c>
@@ -1641,12 +1657,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
@@ -1671,7 +1687,7 @@
       <c r="T8"/>
       <c r="U8"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
@@ -1692,7 +1708,7 @@
       <c r="T9"/>
       <c r="U9"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>140</v>
       </c>
@@ -1717,7 +1733,7 @@
       <c r="T10"/>
       <c r="U10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>140</v>
       </c>
@@ -1738,7 +1754,7 @@
       <c r="T11"/>
       <c r="U11"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>140</v>
       </c>
@@ -1763,12 +1779,12 @@
       <c r="T12"/>
       <c r="U12"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -1791,7 +1807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>140</v>
       </c>
@@ -1810,7 +1826,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
@@ -1829,7 +1845,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
@@ -1852,12 +1868,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>26</v>
       </c>
@@ -1880,7 +1896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
@@ -1899,7 +1915,7 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>140</v>
       </c>
@@ -1918,7 +1934,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>140</v>
       </c>
@@ -1939,12 +1955,12 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>26</v>
       </c>
@@ -1967,7 +1983,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>140</v>
       </c>
@@ -1986,7 +2002,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>140</v>
       </c>
@@ -2005,7 +2021,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>140</v>
       </c>
@@ -2026,16 +2042,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J31" s="24"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
         <v>58</v>
       </c>
       <c r="J32" s="24"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>26</v>
       </c>
@@ -2062,7 +2078,7 @@
       </c>
       <c r="J33" s="24"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>140</v>
       </c>
@@ -2085,7 +2101,7 @@
       <c r="H34" s="1"/>
       <c r="J34" s="24"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>140</v>
       </c>
@@ -2108,7 +2124,7 @@
       <c r="H35" s="1"/>
       <c r="J35" s="24"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>140</v>
       </c>
@@ -2131,7 +2147,7 @@
       <c r="H36" s="1"/>
       <c r="J36" s="24"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>140</v>
       </c>
@@ -2158,7 +2174,7 @@
       </c>
       <c r="J37" s="24"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>140</v>
       </c>
@@ -2185,7 +2201,7 @@
       </c>
       <c r="J38" s="24"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>140</v>
       </c>
@@ -2212,16 +2228,16 @@
       </c>
       <c r="J39" s="24"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J40" s="24"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B41" s="12" t="s">
         <v>61</v>
       </c>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>26</v>
       </c>
@@ -2245,7 +2261,7 @@
       </c>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>140</v>
       </c>
@@ -2265,7 +2281,7 @@
       <c r="G43" s="1"/>
       <c r="J43" s="24"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>140</v>
       </c>
@@ -2284,7 +2300,7 @@
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>140</v>
       </c>
@@ -2307,12 +2323,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B47" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>26</v>
       </c>
@@ -2335,7 +2351,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>140</v>
       </c>
@@ -2354,7 +2370,7 @@
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>140</v>
       </c>
@@ -2373,7 +2389,7 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>140</v>
       </c>
@@ -2397,16 +2413,16 @@
       </c>
       <c r="J51" s="24"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J52" s="24"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B53" s="12" t="s">
         <v>67</v>
       </c>
       <c r="J53" s="24"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>26</v>
       </c>
@@ -2433,7 +2449,7 @@
       </c>
       <c r="J54" s="24"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>140</v>
       </c>
@@ -2456,7 +2472,7 @@
       <c r="H55" s="1"/>
       <c r="J55" s="24"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>140</v>
       </c>
@@ -2479,7 +2495,7 @@
       <c r="H56" s="1"/>
       <c r="J56" s="24"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
@@ -2502,7 +2518,7 @@
       <c r="H57" s="1"/>
       <c r="J57" s="24"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>140</v>
       </c>
@@ -2527,36 +2543,38 @@
       <c r="H58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J58" s="24"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B59" s="1">
+      <c r="J58" s="25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="25">
         <v>20</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1" t="s">
+      <c r="C59" s="25"/>
+      <c r="D59" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="25">
         <v>20</v>
       </c>
-      <c r="G59" s="1">
-        <v>0</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J59" s="25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G59" s="25">
+        <v>0</v>
+      </c>
+      <c r="H59" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J59" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
         <v>137</v>
       </c>
@@ -2583,7 +2601,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
         <v>137</v>
       </c>
@@ -2610,7 +2628,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
         <v>137</v>
       </c>
@@ -2637,16 +2655,16 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J63" s="24"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B64" s="12" t="s">
         <v>68</v>
       </c>
       <c r="J64" s="24"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>26</v>
       </c>
@@ -2670,7 +2688,7 @@
       </c>
       <c r="J65" s="24"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>140</v>
       </c>
@@ -2689,7 +2707,7 @@
       </c>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>140</v>
       </c>
@@ -2708,7 +2726,7 @@
       </c>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>140</v>
       </c>
@@ -2731,12 +2749,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B70" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>26</v>
       </c>
@@ -2762,7 +2780,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="28" t="s">
         <v>140</v>
       </c>
@@ -2788,7 +2806,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>140</v>
       </c>
@@ -2811,7 +2829,7 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>140</v>
       </c>
@@ -2837,7 +2855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>140</v>
       </c>
@@ -2863,7 +2881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>140</v>
       </c>
@@ -2889,55 +2907,57 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B77" s="25">
-        <v>4.0406299999999999E-2</v>
-      </c>
-      <c r="C77" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D77" s="25" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" s="33">
+        <f t="shared" ref="B77:B78" si="0">E77/F77</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C77" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="E77" s="25">
+      <c r="E77" s="32">
         <v>-10000</v>
       </c>
-      <c r="F77" s="25">
+      <c r="F77" s="32">
         <v>20000</v>
       </c>
-      <c r="G77" s="25">
+      <c r="G77" s="32">
         <v>-0.5</v>
       </c>
-      <c r="H77" s="25"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B78" s="25">
-        <v>4.0406299999999999E-2</v>
-      </c>
-      <c r="C78" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D78" s="25" t="s">
+      <c r="H77" s="32"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B78" s="33">
+        <f t="shared" si="0"/>
+        <v>-0.4</v>
+      </c>
+      <c r="C78" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D78" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="E78" s="25">
+      <c r="E78" s="32">
         <v>20000</v>
       </c>
-      <c r="F78" s="25">
+      <c r="F78" s="32">
         <v>-50000</v>
       </c>
-      <c r="G78" s="25">
+      <c r="G78" s="32">
         <v>-0.4</v>
       </c>
-      <c r="H78" s="25"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H78" s="32"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>140</v>
       </c>
@@ -2963,7 +2983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>140</v>
       </c>
@@ -2989,7 +3009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>140</v>
       </c>
@@ -3015,12 +3035,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B83" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
         <v>26</v>
       </c>
@@ -3046,7 +3066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="28" t="s">
         <v>140</v>
       </c>
@@ -3072,7 +3092,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>140</v>
       </c>
@@ -3094,7 +3114,7 @@
       </c>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>140</v>
       </c>
@@ -3117,29 +3137,30 @@
       </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B88" s="25">
-        <v>9.2259999999999998E-4</v>
-      </c>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" s="33">
+        <f>E88/F88</f>
+        <v>6.2500000000000001E-5</v>
+      </c>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="E88" s="25">
+      <c r="E88" s="32">
         <v>5</v>
       </c>
-      <c r="F88" s="25">
+      <c r="F88" s="32">
         <v>80000</v>
       </c>
-      <c r="G88" s="25">
+      <c r="G88" s="32">
         <v>6.2000000000000003E-5</v>
       </c>
-      <c r="H88" s="25"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H88" s="32"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>140</v>
       </c>
@@ -3165,7 +3186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>140</v>
       </c>
@@ -3191,7 +3212,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>140</v>
       </c>
@@ -3217,55 +3238,53 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B92" s="25">
-        <v>0.173903</v>
-      </c>
-      <c r="C92" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D92" s="25" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" s="33">
+        <f t="shared" ref="B92:B93" si="1">E92/F92</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="E92" s="25">
+      <c r="E92" s="32">
         <v>-10000</v>
       </c>
-      <c r="F92" s="25">
+      <c r="F92" s="32">
         <v>20000</v>
       </c>
-      <c r="G92" s="25">
+      <c r="G92" s="32">
         <v>-0.5</v>
       </c>
-      <c r="H92" s="25"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B93" s="25">
-        <v>0.173903</v>
-      </c>
-      <c r="C93" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D93" s="25" t="s">
+      <c r="H92" s="32"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" s="33">
+        <f t="shared" si="1"/>
+        <v>-0.4</v>
+      </c>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="E93" s="25">
+      <c r="E93" s="32">
         <v>20000</v>
       </c>
-      <c r="F93" s="25">
+      <c r="F93" s="32">
         <v>-50000</v>
       </c>
-      <c r="G93" s="25">
+      <c r="G93" s="32">
         <v>-0.4</v>
       </c>
-      <c r="H93" s="25"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H93" s="32"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>140</v>
       </c>
@@ -3291,7 +3310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>140</v>
       </c>
@@ -3317,7 +3336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>140</v>
       </c>
@@ -3343,12 +3362,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B98" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="10" t="s">
         <v>26</v>
       </c>
@@ -3374,12 +3393,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="28" t="s">
         <v>140</v>
       </c>
       <c r="B100" s="28">
-        <v>0.57777780000000001</v>
+        <f>E100/F100</f>
+        <v>9</v>
       </c>
       <c r="C100" s="28"/>
       <c r="D100" s="28" t="s">
@@ -3400,11 +3420,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B101" s="25">
+        <f>E101/F101</f>
         <v>0.25</v>
       </c>
       <c r="C101" s="25"/>
@@ -3421,13 +3442,17 @@
         <v>0</v>
       </c>
       <c r="H101" s="25"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I101" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B102" s="25">
-        <v>3.8168E-3</v>
+        <f>E102/F102</f>
+        <v>1.25E-3</v>
       </c>
       <c r="C102" s="25"/>
       <c r="D102" s="25" t="s">
@@ -3443,8 +3468,11 @@
         <v>0</v>
       </c>
       <c r="H102" s="25"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I102" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>140</v>
       </c>
@@ -3470,7 +3498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>140</v>
       </c>
@@ -3496,7 +3524,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>140</v>
       </c>
@@ -3522,12 +3550,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B106" s="25">
-        <v>6.3829800000000006E-2</v>
+        <f t="shared" ref="B106:B107" si="2">E106/F106</f>
+        <v>-0.5</v>
       </c>
       <c r="C106" s="25" t="s">
         <v>25</v>
@@ -3545,13 +3574,17 @@
         <v>0</v>
       </c>
       <c r="H106" s="25"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I106" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B107" s="25">
-        <v>6.3829800000000006E-2</v>
+        <f t="shared" si="2"/>
+        <v>-0.4</v>
       </c>
       <c r="C107" s="25" t="s">
         <v>25</v>
@@ -3569,8 +3602,11 @@
         <v>0</v>
       </c>
       <c r="H107" s="25"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I107" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>140</v>
       </c>
@@ -3596,7 +3632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>140</v>
       </c>
@@ -3622,7 +3658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>140</v>
       </c>
@@ -3648,12 +3684,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B112" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="10" t="s">
         <v>26</v>
       </c>
@@ -3679,12 +3715,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="28" t="s">
         <v>140</v>
       </c>
       <c r="B114" s="28">
-        <v>2.5862069999999999</v>
+        <f t="shared" ref="B114:B116" si="3">E114/F114</f>
+        <v>9</v>
       </c>
       <c r="C114" s="28"/>
       <c r="D114" s="28" t="s">
@@ -3705,11 +3742,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B115" s="25">
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="C115" s="25"/>
@@ -3726,13 +3764,17 @@
         <v>0</v>
       </c>
       <c r="H115" s="25"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I115" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B116" s="25">
-        <v>2.0833299999999999E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.25E-3</v>
       </c>
       <c r="C116" s="25"/>
       <c r="D116" s="25" t="s">
@@ -3748,8 +3790,11 @@
         <v>0</v>
       </c>
       <c r="H116" s="25"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I116" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>140</v>
       </c>
@@ -3775,7 +3820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>140</v>
       </c>
@@ -3801,7 +3846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>140</v>
       </c>
@@ -3827,12 +3872,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B120" s="25">
-        <v>0.2368421</v>
+        <f t="shared" ref="B120:B121" si="4">E120/F120</f>
+        <v>-0.5</v>
       </c>
       <c r="C120" s="25" t="s">
         <v>25</v>
@@ -3850,13 +3896,17 @@
         <v>0</v>
       </c>
       <c r="H120" s="25"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I120" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B121" s="25">
-        <v>0.2368421</v>
+        <f t="shared" si="4"/>
+        <v>-0.4</v>
       </c>
       <c r="C121" s="25" t="s">
         <v>25</v>
@@ -3874,8 +3924,11 @@
         <v>0</v>
       </c>
       <c r="H121" s="25"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I121" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>140</v>
       </c>
@@ -3901,7 +3954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>140</v>
       </c>
@@ -3927,7 +3980,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>140</v>
       </c>
@@ -3964,21 +4017,21 @@
   <dimension ref="B1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="13"/>
+    <col min="7" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E1" s="21" t="s">
         <v>115</v>
       </c>
@@ -3986,7 +4039,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>83</v>
       </c>
@@ -4003,7 +4056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>97</v>
       </c>
@@ -4020,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>99</v>
       </c>
@@ -4037,7 +4090,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>100</v>
       </c>
@@ -4054,7 +4107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>84</v>
       </c>
@@ -4071,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>102</v>
       </c>
@@ -4088,7 +4141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>85</v>
       </c>
@@ -4105,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>86</v>
       </c>
@@ -4122,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>106</v>
       </c>
@@ -4139,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>108</v>
       </c>
@@ -4156,7 +4209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>117</v>
       </c>
@@ -4173,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>162</v>
       </c>
@@ -4190,7 +4243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>89</v>
       </c>
@@ -4205,7 +4258,7 @@
       </c>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>89</v>
       </c>
@@ -4220,7 +4273,7 @@
       </c>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>89</v>
       </c>
@@ -4235,7 +4288,7 @@
       </c>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
         <v>89</v>
       </c>
@@ -4250,7 +4303,7 @@
       </c>
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>89</v>
       </c>
@@ -4265,7 +4318,7 @@
       </c>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>89</v>
       </c>
@@ -4294,16 +4347,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.88671875" style="3"/>
     <col min="2" max="2" width="68" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="89.42578125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="3"/>
+    <col min="3" max="3" width="46.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="89.44140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
@@ -4317,7 +4370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Modificato file test Ispro e fixati i ko per i 3 indicatori coinvolti
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.monaco\Desktop\ISP\SorgentiGIT\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alberto.collu\client-intesa\earlywarning-pom\Document\test\ESTERE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7680" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="casistiche Indeterm" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="158">
   <si>
     <t>SNDG</t>
   </si>
@@ -544,15 +544,6 @@
     <t>EST000021</t>
   </si>
   <si>
-    <t>EST000001</t>
-  </si>
-  <si>
-    <t>EST000030</t>
-  </si>
-  <si>
-    <t>ko</t>
-  </si>
-  <si>
     <t>EST000033</t>
   </si>
   <si>
@@ -571,15 +562,6 @@
     <t>EST000046</t>
   </si>
   <si>
-    <t>Il Max è 180</t>
-  </si>
-  <si>
-    <t>Il numero di giorni non può essere negativo</t>
-  </si>
-  <si>
-    <t>Note KO</t>
-  </si>
-  <si>
     <t>EST000043</t>
   </si>
   <si>
@@ -616,22 +598,19 @@
     <t>EST000023</t>
   </si>
   <si>
-    <t>EST000019</t>
-  </si>
-  <si>
-    <t>EST000050</t>
-  </si>
-  <si>
     <t>EST000034</t>
   </si>
   <si>
     <t>Exception 2</t>
   </si>
   <si>
-    <t>Il Max è 20</t>
-  </si>
-  <si>
-    <t>forma determinata</t>
+    <t>EST000037</t>
+  </si>
+  <si>
+    <t>EST000040</t>
+  </si>
+  <si>
+    <t>EST000002</t>
   </si>
 </sst>
 </file>
@@ -724,7 +703,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -770,12 +749,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -848,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -913,30 +886,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1267,19 +1243,19 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="31"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1287,13 +1263,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1304,7 +1280,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
@@ -1313,7 +1289,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -1322,7 +1298,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1331,7 +1307,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -1340,7 +1316,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -1349,7 +1325,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>8</v>
@@ -1358,7 +1334,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -1367,13 +1343,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="31" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1381,19 +1357,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -1414,19 +1390,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="112.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="6.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="112.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>4</v>
       </c>
@@ -1434,7 +1410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>5</v>
       </c>
@@ -1442,7 +1418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>19</v>
       </c>
@@ -1450,7 +1426,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>23</v>
       </c>
@@ -1458,7 +1434,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>24</v>
       </c>
@@ -1466,7 +1442,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="17">
         <v>31</v>
       </c>
@@ -1474,7 +1450,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>45</v>
       </c>
@@ -1482,7 +1458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>52</v>
       </c>
@@ -1490,7 +1466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>57</v>
       </c>
@@ -1498,7 +1474,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>176</v>
       </c>
@@ -1506,7 +1482,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
         <v>178</v>
       </c>
@@ -1514,7 +1490,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="17">
         <v>179</v>
       </c>
@@ -1522,7 +1498,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>184</v>
       </c>
@@ -1530,7 +1506,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="17">
         <v>185</v>
       </c>
@@ -1547,33 +1523,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63:J64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="19.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="21" width="9.109375" style="7"/>
+    <col min="9" max="9" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>26</v>
       </c>
@@ -1596,9 +1572,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -1615,9 +1591,9 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1634,9 +1610,9 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1657,12 +1633,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
@@ -1687,9 +1663,9 @@
       <c r="T8"/>
       <c r="U8"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
@@ -1708,9 +1684,9 @@
       <c r="T9"/>
       <c r="U9"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1733,9 +1709,9 @@
       <c r="T10"/>
       <c r="U10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -1754,9 +1730,9 @@
       <c r="T11"/>
       <c r="U11"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1779,12 +1755,12 @@
       <c r="T12"/>
       <c r="U12"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -1807,9 +1783,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -1826,9 +1802,9 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1845,9 +1821,9 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1868,12 +1844,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>26</v>
       </c>
@@ -1896,9 +1872,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1915,9 +1891,9 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -1934,9 +1910,9 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1955,12 +1931,12 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>26</v>
       </c>
@@ -1983,9 +1959,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -2002,9 +1978,9 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -2021,9 +1997,9 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -2042,16 +2018,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J31" s="24"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>58</v>
       </c>
       <c r="J32" s="24"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>26</v>
       </c>
@@ -2078,9 +2054,9 @@
       </c>
       <c r="J33" s="24"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -2101,9 +2077,9 @@
       <c r="H34" s="1"/>
       <c r="J34" s="24"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -2124,9 +2100,9 @@
       <c r="H35" s="1"/>
       <c r="J35" s="24"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -2147,9 +2123,9 @@
       <c r="H36" s="1"/>
       <c r="J36" s="24"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -2174,9 +2150,9 @@
       </c>
       <c r="J37" s="24"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -2201,9 +2177,9 @@
       </c>
       <c r="J38" s="24"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -2228,16 +2204,16 @@
       </c>
       <c r="J39" s="24"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J40" s="24"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>61</v>
       </c>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>26</v>
       </c>
@@ -2261,9 +2237,9 @@
       </c>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -2281,9 +2257,9 @@
       <c r="G43" s="1"/>
       <c r="J43" s="24"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -2300,9 +2276,9 @@
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -2323,12 +2299,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>26</v>
       </c>
@@ -2351,9 +2327,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -2370,9 +2346,9 @@
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -2389,9 +2365,9 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -2413,16 +2389,16 @@
       </c>
       <c r="J51" s="24"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J52" s="24"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
         <v>67</v>
       </c>
       <c r="J53" s="24"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>26</v>
       </c>
@@ -2449,9 +2425,9 @@
       </c>
       <c r="J54" s="24"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B55" s="1">
         <v>180</v>
@@ -2472,9 +2448,9 @@
       <c r="H55" s="1"/>
       <c r="J55" s="24"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B56" s="1">
         <v>80</v>
@@ -2495,9 +2471,9 @@
       <c r="H56" s="1"/>
       <c r="J56" s="24"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B57" s="1">
         <v>30</v>
@@ -2516,11 +2492,11 @@
         <v>30</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="J57" s="24"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J57" s="32"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -2543,128 +2519,118 @@
       <c r="H58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J58" s="25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B59" s="25">
+      <c r="J58" s="34"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="1">
         <v>20</v>
       </c>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E59" s="25" t="s">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F59" s="25">
+      <c r="F59" s="1">
         <v>20</v>
       </c>
-      <c r="G59" s="25">
-        <v>0</v>
-      </c>
-      <c r="H59" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J59" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B60" s="25">
+      <c r="G59" s="1">
+        <v>20</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="J59" s="33"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="1">
         <v>180</v>
       </c>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25" t="s">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E60" s="1">
+        <v>180</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" s="1">
+        <v>180</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="J60" s="33"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" s="1">
+        <v>-10</v>
+      </c>
+      <c r="F61" s="1">
+        <v>20</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J61" s="33"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E60" s="25">
-        <v>180</v>
-      </c>
-      <c r="F60" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G60" s="25">
-        <v>0</v>
-      </c>
-      <c r="H60" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J60" s="26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B61" s="25">
-        <v>0</v>
-      </c>
-      <c r="C61" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="E61" s="25">
-        <v>-10</v>
-      </c>
-      <c r="F61" s="25">
+      <c r="E62" s="1">
         <v>20</v>
       </c>
-      <c r="G61" s="25">
-        <v>20</v>
-      </c>
-      <c r="H61" s="25"/>
-      <c r="J61" s="26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B62" s="25">
-        <v>0</v>
-      </c>
-      <c r="C62" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" s="25">
-        <v>20</v>
-      </c>
-      <c r="F62" s="25">
+      <c r="F62" s="1">
         <v>-50</v>
       </c>
-      <c r="G62" s="25">
-        <v>20</v>
-      </c>
-      <c r="H62" s="25"/>
-      <c r="J62" s="26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J63" s="24"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J62" s="33"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J63" s="32"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="J64" s="24"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J64" s="32"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>26</v>
       </c>
@@ -2688,16 +2654,16 @@
       </c>
       <c r="J65" s="24"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E66" s="1">
         <v>0</v>
@@ -2707,16 +2673,16 @@
       </c>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B67" s="1">
         <v>1</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E67" s="1">
         <v>1</v>
@@ -2726,18 +2692,18 @@
       </c>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B68" s="1">
-        <v>0</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>23</v>
@@ -2749,12 +2715,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B70" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>26</v>
       </c>
@@ -2780,35 +2746,35 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="28">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" s="26">
         <v>0.73400659999999995</v>
       </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28" t="s">
+      <c r="C72" s="26"/>
+      <c r="D72" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="E72" s="28">
+      <c r="E72" s="26">
         <v>180000</v>
       </c>
-      <c r="F72" s="28">
+      <c r="F72" s="26">
         <v>20000</v>
       </c>
-      <c r="G72" s="28">
+      <c r="G72" s="26">
         <v>9</v>
       </c>
-      <c r="H72" s="28"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H72" s="26"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B73" s="1">
         <f>E73/F73</f>
@@ -2816,7 +2782,7 @@
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E73" s="1">
         <v>20000</v>
@@ -2829,11 +2795,11 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" s="27">
+        <v>137</v>
+      </c>
+      <c r="B74" s="25">
         <v>4.0406299999999999E-2</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -2855,18 +2821,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B75" s="27">
+        <v>137</v>
+      </c>
+      <c r="B75" s="25">
         <v>4.0406299999999999E-2</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>23</v>
@@ -2881,18 +2847,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B76" s="27">
+        <v>137</v>
+      </c>
+      <c r="B76" s="25">
         <v>4.0406299999999999E-2</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E76" s="1">
         <v>180000</v>
@@ -2907,68 +2873,68 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="B77" s="33">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" s="30">
         <f t="shared" ref="B77:B78" si="0">E77/F77</f>
         <v>-0.5</v>
       </c>
-      <c r="C77" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D77" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="E77" s="32">
+      <c r="C77" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E77" s="29">
         <v>-10000</v>
       </c>
-      <c r="F77" s="32">
+      <c r="F77" s="29">
         <v>20000</v>
       </c>
-      <c r="G77" s="32">
+      <c r="G77" s="29">
         <v>-0.5</v>
       </c>
-      <c r="H77" s="32"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="B78" s="33">
+      <c r="H77" s="29"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B78" s="30">
         <f t="shared" si="0"/>
         <v>-0.4</v>
       </c>
-      <c r="C78" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D78" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="E78" s="32">
+      <c r="C78" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="E78" s="29">
         <v>20000</v>
       </c>
-      <c r="F78" s="32">
+      <c r="F78" s="29">
         <v>-50000</v>
       </c>
-      <c r="G78" s="32">
+      <c r="G78" s="29">
         <v>-0.4</v>
       </c>
-      <c r="H78" s="32"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H78" s="29"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B79" s="27">
+        <v>137</v>
+      </c>
+      <c r="B79" s="25">
         <v>4.0406299999999999E-2</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E79" s="1">
         <v>20000</v>
@@ -2983,11 +2949,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B80" s="27">
+        <v>137</v>
+      </c>
+      <c r="B80" s="25">
         <v>4.0406299999999999E-2</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -3009,18 +2975,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B81" s="27">
+        <v>137</v>
+      </c>
+      <c r="B81" s="25">
         <v>4.0406299999999999E-2</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E81" s="1">
         <v>0</v>
@@ -3035,12 +3001,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B83" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>26</v>
       </c>
@@ -3066,42 +3032,42 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B85" s="28">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="26">
         <v>1</v>
       </c>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="E85" s="28">
+      <c r="C85" s="26"/>
+      <c r="D85" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E85" s="26">
         <v>180000</v>
       </c>
-      <c r="F85" s="28">
+      <c r="F85" s="26">
         <v>20000</v>
       </c>
-      <c r="G85" s="28">
+      <c r="G85" s="26">
         <v>9</v>
       </c>
-      <c r="H85" s="28"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H85" s="26"/>
+      <c r="I85" s="27"/>
+      <c r="J85" s="27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B86" s="1">
         <v>0.25</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E86" s="1">
         <v>20000</v>
@@ -3114,9 +3080,9 @@
       </c>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B87" s="1">
         <f>E87/F87</f>
@@ -3124,7 +3090,7 @@
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E87" s="1">
         <v>100</v>
@@ -3137,34 +3103,34 @@
       </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="B88" s="33">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B88" s="30">
         <f>E88/F88</f>
         <v>6.2500000000000001E-5</v>
       </c>
-      <c r="C88" s="32"/>
-      <c r="D88" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="E88" s="32">
+      <c r="C88" s="29"/>
+      <c r="D88" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="E88" s="29">
         <v>5</v>
       </c>
-      <c r="F88" s="32">
+      <c r="F88" s="29">
         <v>80000</v>
       </c>
-      <c r="G88" s="32">
+      <c r="G88" s="29">
         <v>6.2000000000000003E-5</v>
       </c>
-      <c r="H88" s="32"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H88" s="29"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B89" s="27">
+        <v>137</v>
+      </c>
+      <c r="B89" s="25">
         <v>0.173903</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -3186,11 +3152,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B90" s="27">
+        <v>137</v>
+      </c>
+      <c r="B90" s="25">
         <v>0.173903</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -3212,18 +3178,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B91" s="27">
+        <v>137</v>
+      </c>
+      <c r="B91" s="25">
         <v>0.173903</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E91" s="1">
         <v>180000</v>
@@ -3238,64 +3204,64 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="B92" s="33">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="30">
         <f t="shared" ref="B92:B93" si="1">E92/F92</f>
         <v>-0.5</v>
       </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="E92" s="32">
+      <c r="C92" s="29"/>
+      <c r="D92" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="E92" s="29">
         <v>-10000</v>
       </c>
-      <c r="F92" s="32">
+      <c r="F92" s="29">
         <v>20000</v>
       </c>
-      <c r="G92" s="32">
+      <c r="G92" s="29">
         <v>-0.5</v>
       </c>
-      <c r="H92" s="32"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="B93" s="33">
+      <c r="H92" s="29"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B93" s="30">
         <f t="shared" si="1"/>
         <v>-0.4</v>
       </c>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32" t="s">
+      <c r="C93" s="29"/>
+      <c r="D93" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="E93" s="32">
+      <c r="E93" s="29">
         <v>20000</v>
       </c>
-      <c r="F93" s="32">
+      <c r="F93" s="29">
         <v>-50000</v>
       </c>
-      <c r="G93" s="32">
+      <c r="G93" s="29">
         <v>-0.4</v>
       </c>
-      <c r="H93" s="32"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H93" s="29"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B94" s="27">
+        <v>137</v>
+      </c>
+      <c r="B94" s="25">
         <v>0.173903</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E94" s="1">
         <v>20000</v>
@@ -3310,11 +3276,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B95" s="27">
+        <v>137</v>
+      </c>
+      <c r="B95" s="25">
         <v>0.173903</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -3336,18 +3302,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B96" s="27">
+        <v>137</v>
+      </c>
+      <c r="B96" s="25">
         <v>0.173903</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E96" s="1">
         <v>0</v>
@@ -3362,12 +3328,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B98" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>26</v>
       </c>
@@ -3393,90 +3359,84 @@
         <v>53</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A100" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B100" s="28">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B100" s="26">
         <f>E100/F100</f>
         <v>9</v>
       </c>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="E100" s="28">
+      <c r="C100" s="26"/>
+      <c r="D100" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="E100" s="26">
         <v>180000</v>
       </c>
-      <c r="F100" s="28">
+      <c r="F100" s="26">
         <v>20000</v>
       </c>
-      <c r="G100" s="28">
+      <c r="G100" s="26">
         <v>9</v>
       </c>
-      <c r="H100" s="28"/>
-      <c r="I100" s="29"/>
-      <c r="J100" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A101" s="25" t="s">
+      <c r="H100" s="26"/>
+      <c r="I100" s="27"/>
+      <c r="J100" s="27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B101" s="25">
         <f>E101/F101</f>
         <v>0.25</v>
       </c>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="E101" s="25">
+      <c r="C101" s="1"/>
+      <c r="D101" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E101" s="1">
         <v>20000</v>
       </c>
-      <c r="F101" s="25">
+      <c r="F101" s="1">
         <v>80000</v>
       </c>
-      <c r="G101" s="25">
-        <v>0</v>
-      </c>
-      <c r="H101" s="25"/>
-      <c r="I101" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A102" s="25" t="s">
+      <c r="G101" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H101" s="1"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B102" s="25">
         <f>E102/F102</f>
         <v>1.25E-3</v>
       </c>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E102" s="25">
+      <c r="C102" s="1"/>
+      <c r="D102" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E102" s="1">
         <v>100</v>
       </c>
-      <c r="F102" s="25">
+      <c r="F102" s="1">
         <v>80000</v>
       </c>
-      <c r="G102" s="25">
-        <v>0</v>
-      </c>
-      <c r="H102" s="25"/>
-      <c r="I102" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G102" s="1">
+        <v>1.25E-3</v>
+      </c>
+      <c r="H102" s="1"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B103" s="27">
+        <v>137</v>
+      </c>
+      <c r="B103" s="25">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -3498,11 +3458,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B104" s="27">
+        <v>137</v>
+      </c>
+      <c r="B104" s="25">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -3524,11 +3484,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B105" s="27">
+        <v>137</v>
+      </c>
+      <c r="B105" s="25">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -3550,74 +3510,68 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" s="25" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B106" s="25">
         <f t="shared" ref="B106:B107" si="2">E106/F106</f>
         <v>-0.5</v>
       </c>
-      <c r="C106" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D106" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="E106" s="25">
+      <c r="C106" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E106" s="1">
         <v>-10000</v>
       </c>
-      <c r="F106" s="25">
+      <c r="F106" s="1">
         <v>20000</v>
       </c>
-      <c r="G106" s="25">
-        <v>0</v>
-      </c>
-      <c r="H106" s="25"/>
-      <c r="I106" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" s="25" t="s">
+      <c r="G106" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="H106" s="1"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B107" s="25">
         <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
-      <c r="C107" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D107" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="E107" s="25">
+      <c r="C107" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E107" s="1">
         <v>20000</v>
       </c>
-      <c r="F107" s="25">
+      <c r="F107" s="1">
         <v>-50000</v>
       </c>
-      <c r="G107" s="25">
-        <v>0</v>
-      </c>
-      <c r="H107" s="25"/>
-      <c r="I107" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G107" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="H107" s="1"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B108" s="27">
+        <v>137</v>
+      </c>
+      <c r="B108" s="25">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E108" s="1">
         <v>20000</v>
@@ -3632,11 +3586,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B109" s="27">
+        <v>137</v>
+      </c>
+      <c r="B109" s="25">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -3658,18 +3612,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B110" s="27">
+        <v>137</v>
+      </c>
+      <c r="B110" s="25">
         <v>6.3829800000000006E-2</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E110" s="1">
         <v>0</v>
@@ -3684,12 +3638,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B112" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>26</v>
       </c>
@@ -3715,90 +3669,84 @@
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A114" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B114" s="28">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B114" s="26">
         <f t="shared" ref="B114:B116" si="3">E114/F114</f>
         <v>9</v>
       </c>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="E114" s="28">
+      <c r="C114" s="26"/>
+      <c r="D114" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E114" s="26">
         <v>180000</v>
       </c>
-      <c r="F114" s="28">
+      <c r="F114" s="26">
         <v>20000</v>
       </c>
-      <c r="G114" s="28">
+      <c r="G114" s="26">
         <v>9</v>
       </c>
-      <c r="H114" s="28"/>
-      <c r="I114" s="29"/>
-      <c r="J114" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A115" s="25" t="s">
+      <c r="H114" s="26"/>
+      <c r="I114" s="27"/>
+      <c r="J114" s="27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B115" s="25">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="C115" s="25"/>
-      <c r="D115" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="E115" s="25">
+      <c r="C115" s="1"/>
+      <c r="D115" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E115" s="1">
         <v>20000</v>
       </c>
-      <c r="F115" s="25">
+      <c r="F115" s="1">
         <v>80000</v>
       </c>
-      <c r="G115" s="25">
-        <v>0</v>
-      </c>
-      <c r="H115" s="25"/>
-      <c r="I115" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A116" s="25" t="s">
+      <c r="G115" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H115" s="1"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B116" s="25">
         <f t="shared" si="3"/>
         <v>1.25E-3</v>
       </c>
-      <c r="C116" s="25"/>
-      <c r="D116" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="E116" s="25">
+      <c r="C116" s="1"/>
+      <c r="D116" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E116" s="1">
         <v>100</v>
       </c>
-      <c r="F116" s="25">
+      <c r="F116" s="1">
         <v>80000</v>
       </c>
-      <c r="G116" s="25">
-        <v>0</v>
-      </c>
-      <c r="H116" s="25"/>
-      <c r="I116" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G116" s="1">
+        <v>1.25E-3</v>
+      </c>
+      <c r="H116" s="1"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B117" s="27">
+        <v>137</v>
+      </c>
+      <c r="B117" s="25">
         <v>0.2368421</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -3820,18 +3768,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B118" s="27">
+        <v>137</v>
+      </c>
+      <c r="B118" s="25">
         <v>0.2368421</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>23</v>
@@ -3846,11 +3794,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B119" s="27">
+        <v>137</v>
+      </c>
+      <c r="B119" s="25">
         <v>0.2368421</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -3872,67 +3820,61 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A120" s="25" t="s">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B120" s="25">
         <f t="shared" ref="B120:B121" si="4">E120/F120</f>
         <v>-0.5</v>
       </c>
-      <c r="C120" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D120" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E120" s="25">
+      <c r="C120" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E120" s="1">
         <v>-10000</v>
       </c>
-      <c r="F120" s="25">
+      <c r="F120" s="1">
         <v>20000</v>
       </c>
-      <c r="G120" s="25">
-        <v>0</v>
-      </c>
-      <c r="H120" s="25"/>
-      <c r="I120" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A121" s="25" t="s">
+      <c r="G120" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="H120" s="1"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B121" s="25">
         <f t="shared" si="4"/>
         <v>-0.4</v>
       </c>
-      <c r="C121" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D121" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E121" s="25">
+      <c r="C121" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E121" s="1">
         <v>20000</v>
       </c>
-      <c r="F121" s="25">
+      <c r="F121" s="1">
         <v>-50000</v>
       </c>
-      <c r="G121" s="25">
-        <v>0</v>
-      </c>
-      <c r="H121" s="25"/>
-      <c r="I121" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G121" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="H121" s="1"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B122" s="27">
+        <v>137</v>
+      </c>
+      <c r="B122" s="25">
         <v>0.2368421</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -3954,18 +3896,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B123" s="27">
+        <v>137</v>
+      </c>
+      <c r="B123" s="25">
         <v>0.2368421</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E123" s="1">
         <v>0</v>
@@ -3980,11 +3922,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B124" s="27">
+        <v>137</v>
+      </c>
+      <c r="B124" s="25">
         <v>0.2368421</v>
       </c>
       <c r="C124" s="1" t="s">
@@ -4016,22 +3958,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="13"/>
+    <col min="7" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E1" s="21" t="s">
         <v>115</v>
       </c>
@@ -4039,7 +3981,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>83</v>
       </c>
@@ -4056,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>97</v>
       </c>
@@ -4073,7 +4015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>99</v>
       </c>
@@ -4083,14 +4025,14 @@
       <c r="D4" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="28">
         <v>84</v>
       </c>
       <c r="F4" s="21">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>100</v>
       </c>
@@ -4100,14 +4042,14 @@
       <c r="D5" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="28">
         <v>12</v>
       </c>
       <c r="F5" s="21">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>84</v>
       </c>
@@ -4124,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>102</v>
       </c>
@@ -4141,7 +4083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>85</v>
       </c>
@@ -4158,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>86</v>
       </c>
@@ -4175,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>106</v>
       </c>
@@ -4192,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>108</v>
       </c>
@@ -4209,7 +4151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>117</v>
       </c>
@@ -4226,9 +4168,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>118</v>
@@ -4243,7 +4185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>89</v>
       </c>
@@ -4258,7 +4200,7 @@
       </c>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>89</v>
       </c>
@@ -4273,7 +4215,7 @@
       </c>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>89</v>
       </c>
@@ -4288,7 +4230,7 @@
       </c>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>89</v>
       </c>
@@ -4303,7 +4245,7 @@
       </c>
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>89</v>
       </c>
@@ -4318,7 +4260,7 @@
       </c>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>89</v>
       </c>
@@ -4328,7 +4270,7 @@
       <c r="D19" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="28">
         <v>1337</v>
       </c>
       <c r="F19" s="21"/>
@@ -4343,20 +4285,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="8.85546875" style="3"/>
     <col min="2" max="2" width="68" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="89.44140625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="46.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="89.42578125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
@@ -4370,7 +4312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
test/ESTERE/test_ind_ISPRO_svil.xlsx aggiunta test IND_8
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
+++ b/earlywarning-pom/Document/test/ESTERE/test_ind_ISPRO_svil.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="172">
   <si>
     <t>SNDG</t>
   </si>
@@ -612,11 +612,57 @@
   <si>
     <t>EST000002</t>
   </si>
+  <si>
+    <t>indicatore 8</t>
+  </si>
+  <si>
+    <t>NUM_IND_8</t>
+  </si>
+  <si>
+    <t>DEN_IND_8</t>
+  </si>
+  <si>
+    <t>IND_TMP_8</t>
+  </si>
+  <si>
+    <t>Tutte Variabili Missing</t>
+  </si>
+  <si>
+    <t>INFLOWS_ACCOUNT_M11 Missing</t>
+  </si>
+  <si>
+    <t>EST000001</t>
+  </si>
+  <si>
+    <t>0.000000</t>
+  </si>
+  <si>
+    <t>Tutte Variabili = 0</t>
+  </si>
+  <si>
+    <t>MISSING</t>
+  </si>
+  <si>
+    <t>EST000006</t>
+  </si>
+  <si>
+    <t>Num = 0</t>
+  </si>
+  <si>
+    <t>Den = 0</t>
+  </si>
+  <si>
+    <t>EST000015</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="171" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="172" formatCode="#,##0.000000"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -821,7 +867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -902,9 +948,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -913,6 +956,31 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1250,10 +1318,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -1344,10 +1412,10 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="31"/>
+      <c r="C14" s="34"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -1521,18 +1589,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U124"/>
+  <dimension ref="A1:U152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63:J64"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="7" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
@@ -2492,7 +2560,7 @@
         <v>30</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="J57" s="32"/>
+      <c r="J57" s="31"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -2519,7 +2587,7 @@
       <c r="H58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J58" s="34"/>
+      <c r="J58" s="33"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -2542,7 +2610,7 @@
         <v>20</v>
       </c>
       <c r="H59" s="1"/>
-      <c r="J59" s="33"/>
+      <c r="J59" s="32"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -2565,7 +2633,7 @@
         <v>180</v>
       </c>
       <c r="H60" s="1"/>
-      <c r="J60" s="33"/>
+      <c r="J60" s="32"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -2592,7 +2660,7 @@
       <c r="H61" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J61" s="33"/>
+      <c r="J61" s="32"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
@@ -2619,16 +2687,16 @@
       <c r="H62" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J62" s="33"/>
+      <c r="J62" s="32"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J63" s="32"/>
+      <c r="J63" s="31"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="J64" s="32"/>
+      <c r="J64" s="31"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
@@ -3643,7 +3711,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>26</v>
       </c>
@@ -3669,7 +3737,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="26" t="s">
         <v>137</v>
       </c>
@@ -3696,7 +3764,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>137</v>
       </c>
@@ -3719,7 +3787,7 @@
       </c>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>137</v>
       </c>
@@ -3742,7 +3810,7 @@
       </c>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>137</v>
       </c>
@@ -3768,7 +3836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>137</v>
       </c>
@@ -3794,7 +3862,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>137</v>
       </c>
@@ -3820,7 +3888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>137</v>
       </c>
@@ -3845,7 +3913,7 @@
       </c>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>137</v>
       </c>
@@ -3870,7 +3938,7 @@
       </c>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>137</v>
       </c>
@@ -3896,7 +3964,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>137</v>
       </c>
@@ -3922,7 +3990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>137</v>
       </c>
@@ -3947,6 +4015,862 @@
       <c r="H124" s="1" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B126" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A127" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D127" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G127" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I127" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J127" s="31"/>
+      <c r="K127" s="31"/>
+      <c r="L127" s="31"/>
+    </row>
+    <row r="128" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B128" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D128" s="22">
+        <v>17962405</v>
+      </c>
+      <c r="E128" s="42">
+        <v>1</v>
+      </c>
+      <c r="F128" s="42">
+        <v>1</v>
+      </c>
+      <c r="G128" s="42">
+        <v>1</v>
+      </c>
+      <c r="H128" s="42">
+        <v>1</v>
+      </c>
+      <c r="I128" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J128" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="K128" s="31"/>
+      <c r="L128" s="31"/>
+      <c r="M128" s="24"/>
+      <c r="N128" s="24"/>
+      <c r="O128" s="24"/>
+      <c r="P128" s="24"/>
+      <c r="Q128" s="24"/>
+      <c r="R128" s="24"/>
+      <c r="S128" s="24"/>
+      <c r="T128" s="24"/>
+      <c r="U128" s="24"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B129" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D129" s="1">
+        <v>26852821</v>
+      </c>
+      <c r="E129" s="42">
+        <v>1</v>
+      </c>
+      <c r="F129" s="42">
+        <v>1</v>
+      </c>
+      <c r="G129" s="42">
+        <v>1</v>
+      </c>
+      <c r="H129" s="42">
+        <v>1</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J129" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="K129" s="31"/>
+      <c r="L129" s="31"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B130" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D130" s="1">
+        <v>26858237</v>
+      </c>
+      <c r="E130" s="42">
+        <v>1</v>
+      </c>
+      <c r="F130" s="42">
+        <v>1</v>
+      </c>
+      <c r="G130" s="42">
+        <v>1</v>
+      </c>
+      <c r="H130" s="42">
+        <v>1</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J130" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="K130" s="31"/>
+      <c r="L130" s="31"/>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B131" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D131" s="1">
+        <v>26858245</v>
+      </c>
+      <c r="E131" s="42">
+        <v>1</v>
+      </c>
+      <c r="F131" s="42">
+        <v>1</v>
+      </c>
+      <c r="G131" s="42">
+        <v>1</v>
+      </c>
+      <c r="H131" s="42">
+        <v>1</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J131" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="K131" s="31"/>
+      <c r="L131" s="31"/>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B132" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D132" s="1">
+        <v>26858269</v>
+      </c>
+      <c r="E132" s="42">
+        <v>1</v>
+      </c>
+      <c r="F132" s="42">
+        <v>1</v>
+      </c>
+      <c r="G132" s="42">
+        <v>1</v>
+      </c>
+      <c r="H132" s="42">
+        <v>1</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J132" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="K132" s="31"/>
+      <c r="L132" s="31"/>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B133" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1">
+        <v>27852861</v>
+      </c>
+      <c r="E133" s="36">
+        <v>219731.77</v>
+      </c>
+      <c r="F133" s="39">
+        <v>200715.582727</v>
+      </c>
+      <c r="G133" s="41">
+        <v>1.0947420000000001</v>
+      </c>
+      <c r="H133" s="41">
+        <v>1.0947420000000001</v>
+      </c>
+      <c r="I133" s="1"/>
+      <c r="J133" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="K133" s="31"/>
+      <c r="L133" s="31"/>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B134" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1">
+        <v>27853140</v>
+      </c>
+      <c r="E134" s="39">
+        <v>6322.5024999999996</v>
+      </c>
+      <c r="F134" s="39">
+        <v>9730.5436360000003</v>
+      </c>
+      <c r="G134" s="1">
+        <v>0.64975799999999995</v>
+      </c>
+      <c r="H134" s="1">
+        <v>0.64975799999999995</v>
+      </c>
+      <c r="I134" s="1"/>
+      <c r="J134" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="K134" s="31"/>
+      <c r="L134" s="31"/>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B135" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1">
+        <v>52866573</v>
+      </c>
+      <c r="E135" s="39">
+        <v>62250.52</v>
+      </c>
+      <c r="F135" s="39">
+        <v>30289.929091000002</v>
+      </c>
+      <c r="G135" s="41">
+        <v>2.0551560000000002</v>
+      </c>
+      <c r="H135" s="41">
+        <v>2.0551560000000002</v>
+      </c>
+      <c r="I135" s="1"/>
+      <c r="J135" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="K135" s="31"/>
+      <c r="L135" s="31"/>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B136" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1">
+        <v>52866675</v>
+      </c>
+      <c r="E136" s="39">
+        <v>519831.34499999997</v>
+      </c>
+      <c r="F136" s="39">
+        <v>375276.09181800002</v>
+      </c>
+      <c r="G136" s="41">
+        <v>1.385197</v>
+      </c>
+      <c r="H136" s="41">
+        <v>1.385197</v>
+      </c>
+      <c r="I136" s="1"/>
+      <c r="J136" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="K136" s="31"/>
+      <c r="L136" s="31"/>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1">
+        <v>68048236</v>
+      </c>
+      <c r="E137" s="39">
+        <v>370365.1</v>
+      </c>
+      <c r="F137" s="39">
+        <v>278663.76909100002</v>
+      </c>
+      <c r="G137" s="41">
+        <v>1.329075</v>
+      </c>
+      <c r="H137" s="41">
+        <v>1.329075</v>
+      </c>
+      <c r="I137" s="1"/>
+      <c r="J137" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="K137" s="31"/>
+      <c r="L137" s="31"/>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B138" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E138" s="40">
+        <v>0</v>
+      </c>
+      <c r="F138" s="40">
+        <v>0</v>
+      </c>
+      <c r="G138" s="41">
+        <v>1</v>
+      </c>
+      <c r="H138" s="41">
+        <v>1</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J138" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="K138" s="31"/>
+      <c r="L138" s="31"/>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B139" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E139" s="40">
+        <v>0</v>
+      </c>
+      <c r="F139" s="40">
+        <v>0</v>
+      </c>
+      <c r="G139" s="41">
+        <v>1</v>
+      </c>
+      <c r="H139" s="41">
+        <v>1</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J139" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="K139" s="31"/>
+      <c r="L139" s="31"/>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B140" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E140" s="40">
+        <v>0</v>
+      </c>
+      <c r="F140" s="40">
+        <v>0</v>
+      </c>
+      <c r="G140" s="41">
+        <v>1</v>
+      </c>
+      <c r="H140" s="41">
+        <v>1</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J140" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="K140" s="31"/>
+      <c r="L140" s="31"/>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E141" s="40">
+        <v>0</v>
+      </c>
+      <c r="F141" s="40">
+        <v>0</v>
+      </c>
+      <c r="G141" s="41">
+        <v>1</v>
+      </c>
+      <c r="H141" s="41">
+        <v>1</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J141" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="K141" s="31"/>
+      <c r="L141" s="31"/>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B142" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E142" s="40">
+        <v>0</v>
+      </c>
+      <c r="F142" s="40">
+        <v>0</v>
+      </c>
+      <c r="G142" s="41">
+        <v>1</v>
+      </c>
+      <c r="H142" s="41">
+        <v>1</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J142" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="K142" s="31"/>
+      <c r="L142" s="31"/>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B143" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E143" s="40">
+        <v>0</v>
+      </c>
+      <c r="F143" s="40">
+        <v>1</v>
+      </c>
+      <c r="G143" s="40">
+        <v>0</v>
+      </c>
+      <c r="H143" s="40">
+        <v>0</v>
+      </c>
+      <c r="I143" s="1"/>
+      <c r="J143" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="K143" s="31"/>
+      <c r="L143" s="31"/>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B144" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E144" s="40">
+        <v>0</v>
+      </c>
+      <c r="F144" s="40">
+        <v>1.3333330000000001</v>
+      </c>
+      <c r="G144" s="40">
+        <v>0</v>
+      </c>
+      <c r="H144" s="40">
+        <v>0</v>
+      </c>
+      <c r="I144" s="1"/>
+      <c r="J144" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="K144" s="31"/>
+      <c r="L144" s="31"/>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B145" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C145" s="1"/>
+      <c r="D145" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E145" s="40">
+        <v>0</v>
+      </c>
+      <c r="F145" s="40">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="G145" s="40">
+        <v>0</v>
+      </c>
+      <c r="H145" s="40">
+        <v>0</v>
+      </c>
+      <c r="I145" s="1"/>
+      <c r="J145" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="K145" s="31"/>
+      <c r="L145" s="31"/>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B146" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E146" s="40">
+        <v>0</v>
+      </c>
+      <c r="F146" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="G146" s="40">
+        <v>0</v>
+      </c>
+      <c r="H146" s="40">
+        <v>0</v>
+      </c>
+      <c r="I146" s="1"/>
+      <c r="J146" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="K146" s="31"/>
+      <c r="L146" s="31"/>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B147" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E147" s="40">
+        <v>0</v>
+      </c>
+      <c r="F147" s="40">
+        <v>1</v>
+      </c>
+      <c r="G147" s="40">
+        <v>0</v>
+      </c>
+      <c r="H147" s="40">
+        <v>0</v>
+      </c>
+      <c r="I147" s="1"/>
+      <c r="J147" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="K147" s="31"/>
+      <c r="L147" s="31"/>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B148" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E148" s="40">
+        <v>5</v>
+      </c>
+      <c r="F148" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="G148" s="40">
+        <v>1</v>
+      </c>
+      <c r="H148" s="40">
+        <v>1</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J148" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K148" s="31"/>
+      <c r="L148" s="31"/>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B149" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E149" s="40">
+        <v>5</v>
+      </c>
+      <c r="F149" s="40">
+        <v>0</v>
+      </c>
+      <c r="G149" s="40">
+        <v>1</v>
+      </c>
+      <c r="H149" s="40">
+        <v>1</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J149" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K149" s="31"/>
+      <c r="L149" s="31"/>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B150" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E150" s="40">
+        <v>5</v>
+      </c>
+      <c r="F150" s="40">
+        <v>0</v>
+      </c>
+      <c r="G150" s="40">
+        <v>1</v>
+      </c>
+      <c r="H150" s="40">
+        <v>1</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J150" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K150" s="31"/>
+      <c r="L150" s="31"/>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B151" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E151" s="40">
+        <v>5</v>
+      </c>
+      <c r="F151" s="40">
+        <v>0</v>
+      </c>
+      <c r="G151" s="40">
+        <v>1</v>
+      </c>
+      <c r="H151" s="40">
+        <v>1</v>
+      </c>
+      <c r="I151" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J151" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K151" s="31"/>
+      <c r="L151" s="31"/>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B152" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E152" s="40">
+        <v>5</v>
+      </c>
+      <c r="F152" s="40">
+        <v>0</v>
+      </c>
+      <c r="G152" s="40">
+        <v>1</v>
+      </c>
+      <c r="H152" s="40">
+        <v>1</v>
+      </c>
+      <c r="I152" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J152" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K152" s="31"/>
+      <c r="L152" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>